<commit_message>
corrected some mistakes with input file
</commit_message>
<xml_diff>
--- a/app/input/input.xlsx
+++ b/app/input/input.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>№ плавки</t>
   </si>
@@ -192,12 +192,6 @@
   </si>
   <si>
     <t>1 зона по ВТР закалка</t>
-  </si>
-  <si>
-    <t>18ХМФБ</t>
-  </si>
-  <si>
-    <t>13ХФА</t>
   </si>
   <si>
     <t>Гр. прочн.</t>
@@ -578,10 +572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BB8"/>
+  <dimension ref="A1:BB7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,7 +612,7 @@
         <v>23</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>58</v>
@@ -782,7 +776,7 @@
         <v>5.51</v>
       </c>
       <c r="K2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L2">
         <v>900</v>
@@ -906,374 +900,10 @@
       </c>
       <c r="BB2">
         <v>14.834143442717471</v>
-      </c>
-    </row>
-    <row r="3" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="D3">
-        <v>0.5</v>
-      </c>
-      <c r="H3" t="s">
-        <v>54</v>
-      </c>
-      <c r="I3">
-        <v>73.02</v>
-      </c>
-      <c r="J3">
-        <v>5.51</v>
-      </c>
-      <c r="K3" t="s">
-        <v>62</v>
-      </c>
-      <c r="L3">
-        <v>900</v>
-      </c>
-      <c r="M3">
-        <v>850</v>
-      </c>
-      <c r="N3">
-        <v>860</v>
-      </c>
-      <c r="O3">
-        <v>1</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="S3">
-        <v>515</v>
-      </c>
-      <c r="T3">
-        <v>515</v>
-      </c>
-      <c r="U3">
-        <v>513</v>
-      </c>
-      <c r="V3">
-        <v>513</v>
-      </c>
-      <c r="W3">
-        <v>514</v>
-      </c>
-      <c r="Y3">
-        <v>24</v>
-      </c>
-      <c r="Z3">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="D4">
-        <v>0.5</v>
-      </c>
-      <c r="H4" t="s">
-        <v>59</v>
-      </c>
-      <c r="I4">
-        <v>73.02</v>
-      </c>
-      <c r="J4">
-        <v>5.51</v>
-      </c>
-      <c r="K4" t="s">
-        <v>62</v>
-      </c>
-      <c r="L4">
-        <v>900</v>
-      </c>
-      <c r="M4">
-        <v>850</v>
-      </c>
-      <c r="N4">
-        <v>860</v>
-      </c>
-      <c r="O4">
-        <v>1</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="S4">
-        <v>515</v>
-      </c>
-      <c r="T4">
-        <v>515</v>
-      </c>
-      <c r="U4">
-        <v>513</v>
-      </c>
-      <c r="V4">
-        <v>513</v>
-      </c>
-      <c r="W4">
-        <v>514</v>
-      </c>
-      <c r="Y4">
-        <v>24</v>
-      </c>
-      <c r="Z4">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="D5">
-        <v>0.5</v>
-      </c>
-      <c r="H5" t="s">
-        <v>59</v>
-      </c>
-      <c r="I5">
-        <v>73.02</v>
-      </c>
-      <c r="J5">
-        <v>5.51</v>
-      </c>
-      <c r="K5" t="s">
-        <v>62</v>
-      </c>
-      <c r="L5">
-        <v>900</v>
-      </c>
-      <c r="M5">
-        <v>850</v>
-      </c>
-      <c r="N5">
-        <v>860</v>
-      </c>
-      <c r="O5">
-        <v>1</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="S5">
-        <v>515</v>
-      </c>
-      <c r="T5">
-        <v>515</v>
-      </c>
-      <c r="U5">
-        <v>513</v>
-      </c>
-      <c r="V5">
-        <v>513</v>
-      </c>
-      <c r="W5">
-        <v>514</v>
-      </c>
-      <c r="Y5">
-        <v>24</v>
-      </c>
-      <c r="Z5">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="D6">
-        <v>0.5</v>
-      </c>
-      <c r="H6" t="s">
-        <v>60</v>
-      </c>
-      <c r="I6">
-        <v>73.02</v>
-      </c>
-      <c r="J6">
-        <v>5.51</v>
-      </c>
-      <c r="K6" t="s">
-        <v>62</v>
-      </c>
-      <c r="L6">
-        <v>900</v>
-      </c>
-      <c r="M6">
-        <v>850</v>
-      </c>
-      <c r="N6">
-        <v>860</v>
-      </c>
-      <c r="O6">
-        <v>1</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="S6">
-        <v>515</v>
-      </c>
-      <c r="T6">
-        <v>515</v>
-      </c>
-      <c r="U6">
-        <v>513</v>
-      </c>
-      <c r="V6">
-        <v>513</v>
-      </c>
-      <c r="W6">
-        <v>514</v>
-      </c>
-      <c r="Y6">
-        <v>24</v>
-      </c>
-      <c r="Z6">
-        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
-    </row>
-    <row r="8" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E8">
-        <v>68.724489795918359</v>
-      </c>
-      <c r="F8">
-        <v>51.020408163265301</v>
-      </c>
-      <c r="G8" t="s">
-        <v>55</v>
-      </c>
-      <c r="I8">
-        <v>73.02</v>
-      </c>
-      <c r="J8">
-        <v>5.51</v>
-      </c>
-      <c r="K8" t="s">
-        <v>62</v>
-      </c>
-      <c r="L8">
-        <v>900</v>
-      </c>
-      <c r="M8">
-        <v>850</v>
-      </c>
-      <c r="N8">
-        <v>860</v>
-      </c>
-      <c r="O8">
-        <v>1</v>
-      </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
-      <c r="S8">
-        <v>515</v>
-      </c>
-      <c r="T8">
-        <v>515</v>
-      </c>
-      <c r="U8">
-        <v>513</v>
-      </c>
-      <c r="V8">
-        <v>513</v>
-      </c>
-      <c r="W8">
-        <v>514</v>
-      </c>
-      <c r="X8">
-        <v>4.5114285714285716</v>
-      </c>
-      <c r="Y8">
-        <v>24</v>
-      </c>
-      <c r="Z8">
-        <v>24</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>56</v>
-      </c>
-      <c r="AB8">
-        <v>0.32</v>
-      </c>
-      <c r="AC8">
-        <v>1.26</v>
-      </c>
-      <c r="AD8">
-        <v>0.34</v>
-      </c>
-      <c r="AE8">
-        <v>0.02</v>
-      </c>
-      <c r="AF8">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="AG8">
-        <v>0.15</v>
-      </c>
-      <c r="AH8">
-        <v>0.12</v>
-      </c>
-      <c r="AI8">
-        <v>0.19</v>
-      </c>
-      <c r="AJ8">
-        <v>0.03</v>
-      </c>
-      <c r="AK8">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="AL8">
-        <v>0.01</v>
-      </c>
-      <c r="AM8">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="AN8">
-        <v>0.02</v>
-      </c>
-      <c r="AO8">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="AP8">
-        <v>0</v>
-      </c>
-      <c r="AQ8">
-        <v>1.7930948762607359</v>
-      </c>
-      <c r="AR8">
-        <v>0.58566666666666678</v>
-      </c>
-      <c r="AS8">
-        <v>839.52000160793887</v>
-      </c>
-      <c r="AT8">
-        <v>15.359181244200631</v>
-      </c>
-      <c r="AU8">
-        <v>49.510675532186497</v>
-      </c>
-      <c r="AV8">
-        <v>8.8897810108672903</v>
-      </c>
-      <c r="AW8">
-        <v>9.1513710699645969</v>
-      </c>
-      <c r="AX8">
-        <v>0.74239049740163332</v>
-      </c>
-      <c r="AY8">
-        <v>855</v>
-      </c>
-      <c r="AZ8">
-        <v>-5.3369209999999994</v>
-      </c>
-      <c r="BA8">
-        <v>-47628.302000000003</v>
-      </c>
-      <c r="BB8">
-        <v>14.834143442717471</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add new predict model
</commit_message>
<xml_diff>
--- a/app/input/input.xlsx
+++ b/app/input/input.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="94">
   <si>
     <t>№ плавки</t>
   </si>
@@ -170,41 +170,140 @@
     <t>Величина зерна</t>
   </si>
   <si>
-    <t>8f4022</t>
-  </si>
-  <si>
-    <t>806169</t>
-  </si>
-  <si>
-    <t>13.06.2018</t>
+    <t>B</t>
+  </si>
+  <si>
+    <t>1 зона по ВТР закалка</t>
+  </si>
+  <si>
+    <t>Гр. прочн.</t>
+  </si>
+  <si>
+    <t>8F4921</t>
+  </si>
+  <si>
+    <t>К50-1</t>
+  </si>
+  <si>
+    <t>704140</t>
+  </si>
+  <si>
+    <t>1402</t>
+  </si>
+  <si>
+    <t>37Г2Ф</t>
+  </si>
+  <si>
+    <t>704143</t>
+  </si>
+  <si>
+    <t>1418</t>
+  </si>
+  <si>
+    <t>607089</t>
+  </si>
+  <si>
+    <t>5154</t>
+  </si>
+  <si>
+    <t>201056</t>
+  </si>
+  <si>
+    <t>40838</t>
   </si>
   <si>
     <t>30Г2</t>
   </si>
   <si>
-    <t>ТУ 21</t>
-  </si>
-  <si>
-    <t>ЭСПК</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>1 зона по ВТР закалка</t>
-  </si>
-  <si>
-    <t>Гр. прочн.</t>
-  </si>
-  <si>
-    <t>N80 тип Q</t>
+    <t>201057</t>
+  </si>
+  <si>
+    <t>201058</t>
+  </si>
+  <si>
+    <t>30677</t>
+  </si>
+  <si>
+    <t>К50-2</t>
+  </si>
+  <si>
+    <t>К50-3</t>
+  </si>
+  <si>
+    <t>К50-4</t>
+  </si>
+  <si>
+    <t>К50-5</t>
+  </si>
+  <si>
+    <t>К50-6</t>
+  </si>
+  <si>
+    <t>К50-7</t>
+  </si>
+  <si>
+    <t>К50-8</t>
+  </si>
+  <si>
+    <t>К50-9</t>
+  </si>
+  <si>
+    <t>К50-10</t>
+  </si>
+  <si>
+    <t>К50-11</t>
+  </si>
+  <si>
+    <t>К50-12</t>
+  </si>
+  <si>
+    <t>611411</t>
+  </si>
+  <si>
+    <t>6f7316</t>
+  </si>
+  <si>
+    <t>13ХФА</t>
+  </si>
+  <si>
+    <t>701345</t>
+  </si>
+  <si>
+    <t>7f0138</t>
+  </si>
+  <si>
+    <t>209176</t>
+  </si>
+  <si>
+    <t>v22400</t>
+  </si>
+  <si>
+    <t>507367</t>
+  </si>
+  <si>
+    <t>5f1246</t>
+  </si>
+  <si>
+    <t>502100</t>
+  </si>
+  <si>
+    <t>5f0640</t>
+  </si>
+  <si>
+    <t>502102</t>
+  </si>
+  <si>
+    <t>5f0642</t>
+  </si>
+  <si>
+    <t>20А-пр</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,6 +318,20 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="3">
@@ -235,7 +348,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -258,19 +371,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -360,7 +497,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -395,7 +531,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -571,245 +706,227 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BB7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:BB14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S17" sqref="S17"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:54" s="6" customFormat="1" ht="120">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="M1" s="2" t="s">
+      <c r="K1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="M1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="U1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="V1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="W1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Y1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="Z1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AB1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AC1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AD1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AE1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AF1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AG1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AH1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AI1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AK1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AL1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AM1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AN1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AO1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AP1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AP1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AQ1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AR1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AS1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AT1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AU1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AV1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AW1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AX1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="AY1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="AZ1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BA1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BB1" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" t="s">
-        <v>53</v>
+    <row r="2" spans="1:54" ht="15.75" thickBot="1">
+      <c r="A2" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="D2">
-        <v>0.5</v>
-      </c>
-      <c r="E2">
-        <v>68.724489795918359</v>
-      </c>
-      <c r="F2">
-        <v>51.020408163265301</v>
-      </c>
-      <c r="G2" t="s">
+        <v>0.2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>93</v>
+      </c>
+      <c r="I2">
+        <v>159</v>
+      </c>
+      <c r="J2">
+        <v>6</v>
+      </c>
+      <c r="K2" t="s">
         <v>55</v>
       </c>
-      <c r="H2" t="s">
-        <v>54</v>
-      </c>
-      <c r="I2">
-        <v>73.02</v>
-      </c>
-      <c r="J2">
-        <v>5.51</v>
-      </c>
-      <c r="K2" t="s">
-        <v>60</v>
-      </c>
       <c r="L2">
-        <v>900</v>
+        <v>865</v>
       </c>
       <c r="M2">
-        <v>850</v>
+        <v>865</v>
       </c>
       <c r="N2">
-        <v>860</v>
+        <v>870</v>
       </c>
       <c r="O2">
-        <v>1</v>
+        <v>0.65</v>
       </c>
       <c r="P2">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="S2">
-        <v>515</v>
+        <v>705</v>
       </c>
       <c r="T2">
-        <v>515</v>
+        <v>705</v>
       </c>
       <c r="U2">
-        <v>513</v>
+        <v>691</v>
       </c>
       <c r="V2">
-        <v>513</v>
+        <v>691</v>
       </c>
       <c r="W2">
-        <v>514</v>
-      </c>
-      <c r="X2">
-        <v>4.5114285714285716</v>
+        <v>676</v>
       </c>
       <c r="Y2">
         <v>24</v>
@@ -817,93 +934,1367 @@
       <c r="Z2">
         <v>24</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" s="2">
+        <v>0.21</v>
+      </c>
+      <c r="AC2" s="2">
+        <v>0.48</v>
+      </c>
+      <c r="AD2" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="AE2" s="2">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="AF2" s="2">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="AG2" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="AH2" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="AI2" s="2">
+        <v>0.19</v>
+      </c>
+      <c r="AJ2" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="AK2" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="AL2" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AM2" s="2">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="AN2" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="AO2" s="3"/>
+      <c r="AP2" s="3"/>
+    </row>
+    <row r="3" spans="1:54">
+      <c r="A3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3">
+        <v>0.2</v>
+      </c>
+      <c r="E3">
+        <v>55.75</v>
+      </c>
+      <c r="F3">
+        <v>42.5</v>
+      </c>
+      <c r="H3" t="s">
+        <v>82</v>
+      </c>
+      <c r="I3">
+        <v>219</v>
+      </c>
+      <c r="J3">
+        <v>18</v>
+      </c>
+      <c r="K3" t="s">
+        <v>55</v>
+      </c>
+      <c r="L3">
+        <v>935</v>
+      </c>
+      <c r="M3">
+        <v>935</v>
+      </c>
+      <c r="N3">
+        <v>945</v>
+      </c>
+      <c r="O3">
+        <v>0.1</v>
+      </c>
+      <c r="P3">
+        <v>45</v>
+      </c>
+      <c r="S3">
+        <v>700</v>
+      </c>
+      <c r="T3">
+        <v>700</v>
+      </c>
+      <c r="U3">
+        <v>687</v>
+      </c>
+      <c r="V3">
+        <v>687</v>
+      </c>
+      <c r="W3">
+        <v>671</v>
+      </c>
+      <c r="Y3">
+        <v>45</v>
+      </c>
+      <c r="Z3">
+        <v>45</v>
+      </c>
+      <c r="AB3">
+        <v>0.15</v>
+      </c>
+      <c r="AC3">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="AD3">
+        <v>0.31</v>
+      </c>
+      <c r="AE3">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="AF3">
+        <v>2E-3</v>
+      </c>
+      <c r="AG3">
+        <v>0.62</v>
+      </c>
+      <c r="AH3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AI3">
+        <v>0.16</v>
+      </c>
+      <c r="AJ3">
+        <v>0.04</v>
+      </c>
+      <c r="AK3">
+        <v>0.05</v>
+      </c>
+      <c r="AL3">
+        <v>0</v>
+      </c>
+      <c r="AM3">
+        <v>2E-3</v>
+      </c>
+      <c r="AN3">
+        <v>0.03</v>
+      </c>
+      <c r="AO3">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="AP3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:54">
+      <c r="A4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4">
+        <v>0.2</v>
+      </c>
+      <c r="E4">
+        <v>56.25</v>
+      </c>
+      <c r="F4">
+        <v>42.25</v>
+      </c>
+      <c r="H4" t="s">
+        <v>82</v>
+      </c>
+      <c r="I4">
+        <v>219</v>
+      </c>
+      <c r="J4">
+        <v>18</v>
+      </c>
+      <c r="K4" t="s">
+        <v>69</v>
+      </c>
+      <c r="L4">
+        <v>935</v>
+      </c>
+      <c r="M4">
+        <v>935</v>
+      </c>
+      <c r="N4">
+        <v>945</v>
+      </c>
+      <c r="O4">
+        <v>0.1</v>
+      </c>
+      <c r="P4">
+        <v>55</v>
+      </c>
+      <c r="S4">
+        <v>680</v>
+      </c>
+      <c r="T4">
+        <v>680</v>
+      </c>
+      <c r="U4">
+        <v>668</v>
+      </c>
+      <c r="V4">
+        <v>668</v>
+      </c>
+      <c r="W4">
+        <v>652</v>
+      </c>
+      <c r="Y4">
+        <v>40</v>
+      </c>
+      <c r="Z4">
+        <v>40</v>
+      </c>
+      <c r="AB4">
+        <v>0.13</v>
+      </c>
+      <c r="AC4">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="AD4">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="AE4">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="AF4">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="AG4">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="AH4">
+        <v>0.09</v>
+      </c>
+      <c r="AI4">
+        <v>0.19</v>
+      </c>
+      <c r="AJ4">
+        <v>0.05</v>
+      </c>
+      <c r="AK4">
+        <v>0.05</v>
+      </c>
+      <c r="AL4">
+        <v>0</v>
+      </c>
+      <c r="AM4">
+        <v>2E-3</v>
+      </c>
+      <c r="AN4">
+        <v>0</v>
+      </c>
+      <c r="AO4">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="AP4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:54">
+      <c r="A5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5">
+        <v>0.5</v>
+      </c>
+      <c r="E5">
+        <v>77.397959183673464</v>
+      </c>
+      <c r="F5">
+        <v>64.08163265306122</v>
+      </c>
+      <c r="H5" t="s">
+        <v>65</v>
+      </c>
+      <c r="I5">
+        <v>88.9</v>
+      </c>
+      <c r="J5">
+        <v>12.2</v>
+      </c>
+      <c r="K5" t="s">
+        <v>70</v>
+      </c>
+      <c r="L5">
+        <v>900</v>
+      </c>
+      <c r="M5">
+        <v>900</v>
+      </c>
+      <c r="N5">
+        <v>910</v>
+      </c>
+      <c r="O5">
+        <v>0.1</v>
+      </c>
+      <c r="P5">
+        <v>24.6</v>
+      </c>
+      <c r="S5">
+        <v>575</v>
+      </c>
+      <c r="T5">
+        <v>575</v>
+      </c>
+      <c r="U5">
+        <v>571</v>
+      </c>
+      <c r="V5">
+        <v>569</v>
+      </c>
+      <c r="W5">
+        <v>562.20000000000005</v>
+      </c>
+      <c r="Y5">
+        <v>40</v>
+      </c>
+      <c r="Z5">
+        <v>27</v>
+      </c>
+      <c r="AB5">
+        <v>0.27</v>
+      </c>
+      <c r="AC5">
+        <v>1.31</v>
+      </c>
+      <c r="AD5">
+        <v>0.22</v>
+      </c>
+      <c r="AE5">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="AF5">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="AG5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AH5">
+        <v>0.06</v>
+      </c>
+      <c r="AI5">
+        <v>0.09</v>
+      </c>
+      <c r="AJ5">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="AK5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="AL5">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="AM5">
+        <v>0</v>
+      </c>
+      <c r="AN5">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="AO5">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="AP5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:54">
+      <c r="A6" t="s">
         <v>56</v>
       </c>
-      <c r="AB2">
-        <v>0.32</v>
-      </c>
-      <c r="AC2">
-        <v>1.26</v>
-      </c>
-      <c r="AD2">
+      <c r="B6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6">
+        <v>0.2</v>
+      </c>
+      <c r="E6">
+        <v>79.5</v>
+      </c>
+      <c r="F6">
+        <v>67.5</v>
+      </c>
+      <c r="H6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I6">
+        <v>194.5</v>
+      </c>
+      <c r="J6">
+        <v>14.5</v>
+      </c>
+      <c r="K6" t="s">
+        <v>71</v>
+      </c>
+      <c r="L6">
+        <v>880</v>
+      </c>
+      <c r="M6">
+        <v>880</v>
+      </c>
+      <c r="N6">
+        <v>890</v>
+      </c>
+      <c r="O6">
+        <v>0.1</v>
+      </c>
+      <c r="P6">
+        <v>45</v>
+      </c>
+      <c r="S6">
+        <v>685</v>
+      </c>
+      <c r="T6">
+        <v>695</v>
+      </c>
+      <c r="U6">
+        <v>672.642857142857</v>
+      </c>
+      <c r="V6">
+        <v>682</v>
+      </c>
+      <c r="W6">
+        <v>655.142857142857</v>
+      </c>
+      <c r="Y6">
+        <v>40</v>
+      </c>
+      <c r="Z6">
+        <v>40</v>
+      </c>
+      <c r="AB6">
+        <v>0.36</v>
+      </c>
+      <c r="AC6">
+        <v>1.58</v>
+      </c>
+      <c r="AD6">
+        <v>0.24</v>
+      </c>
+      <c r="AE6">
+        <v>1.2E-2</v>
+      </c>
+      <c r="AF6">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="AG6">
+        <v>0.12</v>
+      </c>
+      <c r="AH6">
+        <v>0.08</v>
+      </c>
+      <c r="AI6">
+        <v>0.23</v>
+      </c>
+      <c r="AJ6">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AK6">
+        <v>0.107</v>
+      </c>
+      <c r="AL6">
+        <v>0</v>
+      </c>
+      <c r="AM6">
+        <v>0</v>
+      </c>
+      <c r="AN6">
+        <v>0</v>
+      </c>
+      <c r="AO6">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="AP6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:54">
+      <c r="A7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7">
+        <v>0.2</v>
+      </c>
+      <c r="E7">
+        <v>76</v>
+      </c>
+      <c r="F7">
+        <v>65</v>
+      </c>
+      <c r="H7" t="s">
+        <v>58</v>
+      </c>
+      <c r="I7">
+        <v>194.5</v>
+      </c>
+      <c r="J7">
+        <v>14.5</v>
+      </c>
+      <c r="K7" t="s">
+        <v>72</v>
+      </c>
+      <c r="L7">
+        <v>880</v>
+      </c>
+      <c r="M7">
+        <v>880</v>
+      </c>
+      <c r="N7">
+        <v>890</v>
+      </c>
+      <c r="O7">
+        <v>0.1</v>
+      </c>
+      <c r="P7">
+        <v>45</v>
+      </c>
+      <c r="S7">
+        <v>705</v>
+      </c>
+      <c r="T7">
+        <v>705</v>
+      </c>
+      <c r="U7">
+        <v>682</v>
+      </c>
+      <c r="V7">
+        <v>691</v>
+      </c>
+      <c r="W7">
+        <v>666</v>
+      </c>
+      <c r="Y7">
+        <v>40</v>
+      </c>
+      <c r="Z7">
+        <v>40</v>
+      </c>
+      <c r="AB7">
+        <v>0.36</v>
+      </c>
+      <c r="AC7">
+        <v>1.66</v>
+      </c>
+      <c r="AD7">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="AE7">
+        <v>1.4E-2</v>
+      </c>
+      <c r="AF7">
+        <v>0.01</v>
+      </c>
+      <c r="AG7">
+        <v>0.12</v>
+      </c>
+      <c r="AH7">
+        <v>0.08</v>
+      </c>
+      <c r="AI7">
+        <v>0.22</v>
+      </c>
+      <c r="AJ7">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="AK7">
+        <v>0.113</v>
+      </c>
+      <c r="AL7">
+        <v>0</v>
+      </c>
+      <c r="AM7">
+        <v>0</v>
+      </c>
+      <c r="AN7">
+        <v>0</v>
+      </c>
+      <c r="AO7">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="AP7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:54">
+      <c r="A8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8">
+        <v>0.2</v>
+      </c>
+      <c r="E8">
+        <v>83</v>
+      </c>
+      <c r="F8">
+        <v>79.5</v>
+      </c>
+      <c r="H8" t="s">
+        <v>58</v>
+      </c>
+      <c r="I8">
+        <v>194.5</v>
+      </c>
+      <c r="J8">
+        <v>19.7</v>
+      </c>
+      <c r="K8" t="s">
+        <v>73</v>
+      </c>
+      <c r="L8">
+        <v>880</v>
+      </c>
+      <c r="M8">
+        <v>880</v>
+      </c>
+      <c r="N8">
+        <v>890</v>
+      </c>
+      <c r="O8">
+        <v>0.1</v>
+      </c>
+      <c r="P8">
+        <v>45</v>
+      </c>
+      <c r="S8">
+        <v>645</v>
+      </c>
+      <c r="T8">
+        <v>675</v>
+      </c>
+      <c r="U8">
+        <v>634.7692307692306</v>
+      </c>
+      <c r="V8">
+        <v>663</v>
+      </c>
+      <c r="W8">
+        <v>620.69230769230774</v>
+      </c>
+      <c r="Y8">
+        <v>40</v>
+      </c>
+      <c r="Z8">
+        <v>40</v>
+      </c>
+      <c r="AB8">
+        <v>0.35</v>
+      </c>
+      <c r="AC8">
+        <v>1.61</v>
+      </c>
+      <c r="AD8">
+        <v>0.22</v>
+      </c>
+      <c r="AE8">
+        <v>1.2E-2</v>
+      </c>
+      <c r="AF8">
+        <v>0.01</v>
+      </c>
+      <c r="AG8">
+        <v>0.11</v>
+      </c>
+      <c r="AH8">
+        <v>0.11</v>
+      </c>
+      <c r="AI8">
+        <v>0.24</v>
+      </c>
+      <c r="AJ8">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="AK8">
+        <v>0.108</v>
+      </c>
+      <c r="AL8">
+        <v>0</v>
+      </c>
+      <c r="AM8">
+        <v>0</v>
+      </c>
+      <c r="AN8">
+        <v>0</v>
+      </c>
+      <c r="AO8">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="AP8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:54">
+      <c r="A9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D9">
+        <v>0.2</v>
+      </c>
+      <c r="E9">
+        <v>80.5</v>
+      </c>
+      <c r="F9">
+        <v>70.5</v>
+      </c>
+      <c r="H9" t="s">
+        <v>58</v>
+      </c>
+      <c r="I9">
+        <v>187.7</v>
+      </c>
+      <c r="J9">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="K9" t="s">
+        <v>74</v>
+      </c>
+      <c r="L9">
+        <v>880</v>
+      </c>
+      <c r="M9">
+        <v>880</v>
+      </c>
+      <c r="N9">
+        <v>890</v>
+      </c>
+      <c r="O9">
+        <v>0.1</v>
+      </c>
+      <c r="P9">
+        <v>42.5</v>
+      </c>
+      <c r="S9">
+        <v>680</v>
+      </c>
+      <c r="T9">
+        <v>680</v>
+      </c>
+      <c r="U9">
+        <v>668</v>
+      </c>
+      <c r="V9">
+        <v>668</v>
+      </c>
+      <c r="W9">
+        <v>652</v>
+      </c>
+      <c r="Y9">
+        <v>43.333333333333343</v>
+      </c>
+      <c r="Z9">
+        <v>40</v>
+      </c>
+      <c r="AB9">
+        <v>0.36</v>
+      </c>
+      <c r="AC9">
+        <v>1.53</v>
+      </c>
+      <c r="AD9">
         <v>0.34</v>
       </c>
-      <c r="AE2">
+      <c r="AE9">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="AF9">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="AG9">
+        <v>0.15</v>
+      </c>
+      <c r="AH9">
+        <v>0.13</v>
+      </c>
+      <c r="AI9">
+        <v>0.18</v>
+      </c>
+      <c r="AJ9">
+        <v>0.03</v>
+      </c>
+      <c r="AK9">
+        <v>0.09</v>
+      </c>
+      <c r="AL9">
+        <v>0</v>
+      </c>
+      <c r="AM9">
+        <v>0</v>
+      </c>
+      <c r="AN9">
+        <v>0</v>
+      </c>
+      <c r="AO9">
+        <v>1.2E-2</v>
+      </c>
+      <c r="AP9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:54">
+      <c r="A10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10">
+        <v>0.2</v>
+      </c>
+      <c r="E10">
+        <v>79</v>
+      </c>
+      <c r="F10">
+        <v>67</v>
+      </c>
+      <c r="H10" t="s">
+        <v>58</v>
+      </c>
+      <c r="I10">
+        <v>187.7</v>
+      </c>
+      <c r="J10">
+        <v>23.5</v>
+      </c>
+      <c r="K10" t="s">
+        <v>75</v>
+      </c>
+      <c r="L10">
+        <v>880</v>
+      </c>
+      <c r="M10">
+        <v>880</v>
+      </c>
+      <c r="N10">
+        <v>890</v>
+      </c>
+      <c r="O10">
+        <v>0.1</v>
+      </c>
+      <c r="P10">
+        <v>45</v>
+      </c>
+      <c r="S10">
+        <v>685</v>
+      </c>
+      <c r="T10">
+        <v>685</v>
+      </c>
+      <c r="U10">
+        <v>673</v>
+      </c>
+      <c r="V10">
+        <v>673</v>
+      </c>
+      <c r="W10">
+        <v>666</v>
+      </c>
+      <c r="Y10">
+        <v>45</v>
+      </c>
+      <c r="Z10">
+        <v>45</v>
+      </c>
+      <c r="AB10">
+        <v>0.37</v>
+      </c>
+      <c r="AC10">
+        <v>1.42</v>
+      </c>
+      <c r="AD10">
+        <v>0.31</v>
+      </c>
+      <c r="AE10">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="AF10">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AG10">
+        <v>0.12</v>
+      </c>
+      <c r="AH10">
+        <v>0.13</v>
+      </c>
+      <c r="AI10">
+        <v>0.18</v>
+      </c>
+      <c r="AJ10">
         <v>0.02</v>
       </c>
-      <c r="AF2">
+      <c r="AK10">
+        <v>0.08</v>
+      </c>
+      <c r="AL10">
+        <v>0</v>
+      </c>
+      <c r="AM10">
+        <v>0</v>
+      </c>
+      <c r="AN10">
+        <v>0</v>
+      </c>
+      <c r="AO10">
+        <v>0.01</v>
+      </c>
+      <c r="AP10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:54">
+      <c r="A11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D11">
+        <v>0.2</v>
+      </c>
+      <c r="E11">
+        <v>77</v>
+      </c>
+      <c r="F11">
+        <v>69</v>
+      </c>
+      <c r="H11" t="s">
+        <v>58</v>
+      </c>
+      <c r="I11">
+        <v>187.7</v>
+      </c>
+      <c r="J11">
+        <v>23.5</v>
+      </c>
+      <c r="K11" t="s">
+        <v>76</v>
+      </c>
+      <c r="L11">
+        <v>880</v>
+      </c>
+      <c r="M11">
+        <v>880</v>
+      </c>
+      <c r="N11">
+        <v>890</v>
+      </c>
+      <c r="O11">
+        <v>0.1</v>
+      </c>
+      <c r="P11">
+        <v>45</v>
+      </c>
+      <c r="S11">
+        <v>685</v>
+      </c>
+      <c r="T11">
+        <v>685</v>
+      </c>
+      <c r="U11">
+        <v>673</v>
+      </c>
+      <c r="V11">
+        <v>673</v>
+      </c>
+      <c r="W11">
+        <v>656</v>
+      </c>
+      <c r="Y11">
+        <v>45</v>
+      </c>
+      <c r="Z11">
+        <v>45</v>
+      </c>
+      <c r="AB11">
+        <v>0.36</v>
+      </c>
+      <c r="AC11">
+        <v>1.46</v>
+      </c>
+      <c r="AD11">
+        <v>0.3</v>
+      </c>
+      <c r="AE11">
+        <v>0.01</v>
+      </c>
+      <c r="AF11">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="AG11">
+        <v>0.16</v>
+      </c>
+      <c r="AH11">
+        <v>0.19</v>
+      </c>
+      <c r="AI11">
+        <v>0.22</v>
+      </c>
+      <c r="AJ11">
+        <v>0.02</v>
+      </c>
+      <c r="AK11">
+        <v>0.08</v>
+      </c>
+      <c r="AL11">
+        <v>0</v>
+      </c>
+      <c r="AM11">
+        <v>0</v>
+      </c>
+      <c r="AN11">
+        <v>0</v>
+      </c>
+      <c r="AO11">
+        <v>0.01</v>
+      </c>
+      <c r="AP11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:54">
+      <c r="A12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12">
+        <v>0.5</v>
+      </c>
+      <c r="E12">
+        <v>82.959183673469383</v>
+      </c>
+      <c r="F12">
+        <v>71.326530612244895</v>
+      </c>
+      <c r="H12" t="s">
+        <v>65</v>
+      </c>
+      <c r="I12">
+        <v>88.9</v>
+      </c>
+      <c r="J12">
+        <v>12.2</v>
+      </c>
+      <c r="K12" t="s">
+        <v>77</v>
+      </c>
+      <c r="L12">
+        <v>900</v>
+      </c>
+      <c r="M12">
+        <v>900</v>
+      </c>
+      <c r="N12">
+        <v>910</v>
+      </c>
+      <c r="O12">
+        <v>0.1</v>
+      </c>
+      <c r="P12">
+        <v>40.166666666666657</v>
+      </c>
+      <c r="S12">
+        <v>575.57142857142856</v>
+      </c>
+      <c r="T12">
+        <v>565</v>
+      </c>
+      <c r="U12">
+        <v>569.857142857143</v>
+      </c>
+      <c r="V12">
+        <v>560</v>
+      </c>
+      <c r="W12">
+        <v>559.71428571428567</v>
+      </c>
+      <c r="Y12">
+        <v>40</v>
+      </c>
+      <c r="Z12">
+        <v>27</v>
+      </c>
+      <c r="AB12">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="AC12">
+        <v>1.3</v>
+      </c>
+      <c r="AD12">
+        <v>0.24</v>
+      </c>
+      <c r="AE12">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="AG2">
-        <v>0.15</v>
-      </c>
-      <c r="AH2">
-        <v>0.12</v>
-      </c>
-      <c r="AI2">
-        <v>0.19</v>
-      </c>
-      <c r="AJ2">
-        <v>0.03</v>
-      </c>
-      <c r="AK2">
+      <c r="AF12">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="AG12">
+        <v>0.08</v>
+      </c>
+      <c r="AH12">
+        <v>0.04</v>
+      </c>
+      <c r="AI12">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AJ12">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="AK12">
+        <v>2E-3</v>
+      </c>
+      <c r="AL12">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="AM12">
+        <v>0</v>
+      </c>
+      <c r="AN12">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="AO12">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="AP12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:54">
+      <c r="A13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13">
+        <v>0.5</v>
+      </c>
+      <c r="E13">
+        <v>85.051020408163254</v>
+      </c>
+      <c r="F13">
+        <v>73.724489795918359</v>
+      </c>
+      <c r="H13" t="s">
+        <v>65</v>
+      </c>
+      <c r="I13">
+        <v>88.9</v>
+      </c>
+      <c r="J13">
+        <v>12.2</v>
+      </c>
+      <c r="K13" t="s">
+        <v>78</v>
+      </c>
+      <c r="L13">
+        <v>900</v>
+      </c>
+      <c r="M13">
+        <v>900</v>
+      </c>
+      <c r="N13">
+        <v>910</v>
+      </c>
+      <c r="O13">
+        <v>0.1</v>
+      </c>
+      <c r="P13">
+        <v>39.75</v>
+      </c>
+      <c r="S13">
+        <v>565</v>
+      </c>
+      <c r="T13">
+        <v>565</v>
+      </c>
+      <c r="U13">
+        <v>560</v>
+      </c>
+      <c r="V13">
+        <v>560</v>
+      </c>
+      <c r="W13">
+        <v>551</v>
+      </c>
+      <c r="Y13">
+        <v>40</v>
+      </c>
+      <c r="Z13">
+        <v>27</v>
+      </c>
+      <c r="AB13">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="AC13">
+        <v>1.3</v>
+      </c>
+      <c r="AD13">
+        <v>0.24</v>
+      </c>
+      <c r="AE13">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="AF13">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="AG13">
+        <v>0.08</v>
+      </c>
+      <c r="AH13">
+        <v>0.04</v>
+      </c>
+      <c r="AI13">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AJ13">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="AK13">
+        <v>2E-3</v>
+      </c>
+      <c r="AL13">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="AM13">
+        <v>0</v>
+      </c>
+      <c r="AN13">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="AO13">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="AP13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:54">
+      <c r="A14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14">
+        <v>0.5</v>
+      </c>
+      <c r="E14">
+        <v>84.387755102040813</v>
+      </c>
+      <c r="F14">
+        <v>71.224489795918359</v>
+      </c>
+      <c r="H14" t="s">
+        <v>65</v>
+      </c>
+      <c r="I14">
+        <v>88.9</v>
+      </c>
+      <c r="J14">
+        <v>12.2</v>
+      </c>
+      <c r="K14" t="s">
+        <v>79</v>
+      </c>
+      <c r="L14">
+        <v>900</v>
+      </c>
+      <c r="M14">
+        <v>900</v>
+      </c>
+      <c r="N14">
+        <v>910</v>
+      </c>
+      <c r="O14">
+        <v>0.1</v>
+      </c>
+      <c r="P14">
+        <v>39.333333333333343</v>
+      </c>
+      <c r="S14">
+        <v>565</v>
+      </c>
+      <c r="T14">
+        <v>565</v>
+      </c>
+      <c r="U14">
+        <v>560</v>
+      </c>
+      <c r="V14">
+        <v>560</v>
+      </c>
+      <c r="W14">
+        <v>551</v>
+      </c>
+      <c r="Y14">
+        <v>40</v>
+      </c>
+      <c r="Z14">
+        <v>27</v>
+      </c>
+      <c r="AB14">
+        <v>0.27</v>
+      </c>
+      <c r="AC14">
+        <v>1.36</v>
+      </c>
+      <c r="AD14">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="AE14">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="AF14">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="AG14">
+        <v>0.08</v>
+      </c>
+      <c r="AH14">
+        <v>0.04</v>
+      </c>
+      <c r="AI14">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AJ14">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AK14">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="AL14">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="AM14">
+        <v>0</v>
+      </c>
+      <c r="AN14">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AL2">
-        <v>0.01</v>
-      </c>
-      <c r="AM2">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="AN2">
-        <v>0.02</v>
-      </c>
-      <c r="AO2">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="AP2">
-        <v>0</v>
-      </c>
-      <c r="AQ2">
-        <v>1.7930948762607359</v>
-      </c>
-      <c r="AR2">
-        <v>0.58566666666666678</v>
-      </c>
-      <c r="AS2">
-        <v>839.52000160793887</v>
-      </c>
-      <c r="AT2">
-        <v>15.359181244200631</v>
-      </c>
-      <c r="AU2">
-        <v>49.510675532186497</v>
-      </c>
-      <c r="AV2">
-        <v>8.8897810108672903</v>
-      </c>
-      <c r="AW2">
-        <v>9.1513710699645969</v>
-      </c>
-      <c r="AX2">
-        <v>0.74239049740163332</v>
-      </c>
-      <c r="AY2">
-        <v>855</v>
-      </c>
-      <c r="AZ2">
-        <v>-5.3369209999999994</v>
-      </c>
-      <c r="BA2">
-        <v>-47628.302000000003</v>
-      </c>
-      <c r="BB2">
-        <v>14.834143442717471</v>
-      </c>
-    </row>
-    <row r="7" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
+      <c r="AO14">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="AP14">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>